<commit_message>
Update RP.xlsx with latest data
The RP.xlsx file has been updated. This may include new or modified data, formulas, or formatting changes.
</commit_message>
<xml_diff>
--- a/RP.xlsx
+++ b/RP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443F1FB2-3929-4559-A87E-7CC3A5C7E5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F26BBA9-B7B2-48CD-A5E0-6908617B87C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,13 +186,13 @@
     <t>Waiting to be submitted by Sir</t>
   </si>
   <si>
-    <t>Minor Revision</t>
-  </si>
-  <si>
     <t>Working on it</t>
   </si>
   <si>
     <t>C1,C2 Posterior Temporary Fixation</t>
+  </si>
+  <si>
+    <t>Submitted after Minor Revision</t>
   </si>
 </sst>
 </file>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1"/>
@@ -872,7 +872,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" customHeight="1">
@@ -1037,7 +1037,7 @@
         <v>38</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="24.6" customHeight="1">
@@ -1045,10 +1045,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3">

</xml_diff>